<commit_message>
Update nest hardware doc
</commit_message>
<xml_diff>
--- a/src/downloads/Nest-BOM.xlsx
+++ b/src/downloads/Nest-BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcalc\UCL Dropbox\Lorenza Calcaterra\Project_aeon\Assembly instructions\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B439C2D-EE2E-4D23-B831-798ACB2F6BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5D1293-0F5F-4E15-9A16-F81ACFF06D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38A5E6C9-8D94-40D2-9BFA-B29F5FB44878}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arena" sheetId="1" r:id="rId1"/>
+    <sheet name="AEON nest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,49 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Lorenza Calcaterra</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{D6B7B53A-74D1-435A-80A1-9DCB5D789D63}">
-      <text/>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{9E89FBD3-8EFA-4C5C-9AFB-E97485ABACDC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{578D3F03-C970-4E7D-8407-C2284F8A3500}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t xml:space="preserve">Inventory list </t>
   </si>
@@ -118,12 +77,6 @@
     <t xml:space="preserve">Aluminum extrusion </t>
   </si>
   <si>
-    <t>Arena Frame</t>
-  </si>
-  <si>
-    <t>389-9819</t>
-  </si>
-  <si>
     <t>Bosch Rexroth/RS</t>
   </si>
   <si>
@@ -140,6 +93,72 @@
   </si>
   <si>
     <t>Electronics</t>
+  </si>
+  <si>
+    <t>493-8252</t>
+  </si>
+  <si>
+    <t>281-136</t>
+  </si>
+  <si>
+    <t>232-8451</t>
+  </si>
+  <si>
+    <t>Metal frame</t>
+  </si>
+  <si>
+    <t>Acrylic</t>
+  </si>
+  <si>
+    <t>Acrylic red tinted 5mm</t>
+  </si>
+  <si>
+    <t>Acrylic white matt 3mm</t>
+  </si>
+  <si>
+    <t>Acrylic white matt 5mm</t>
+  </si>
+  <si>
+    <t>Acrylic clear 2mm</t>
+  </si>
+  <si>
+    <t>Direct Plastics</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>bag of 50</t>
+  </si>
+  <si>
+    <t>Cap screw M6 25mm</t>
+  </si>
+  <si>
+    <t>4 screws and 4 insertion nuts included</t>
+  </si>
+  <si>
+    <t>Countersunk screw M6 12mm</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Countersunk screw</t>
+  </si>
+  <si>
+    <t>Cap screw</t>
+  </si>
+  <si>
+    <t>Cap screw M6 50mm</t>
+  </si>
+  <si>
+    <t>293-404</t>
+  </si>
+  <si>
+    <t>3D printer</t>
+  </si>
+  <si>
+    <t>3D printed material</t>
   </si>
 </sst>
 </file>
@@ -149,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,22 +221,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -247,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,9 +282,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -295,7 +299,37 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -462,7 +496,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}" name="Table2" displayName="Table2" ref="A3:J43" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}" name="Table2" displayName="Table2" ref="A3:J43" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A3:J43" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{B4854CC6-A69E-4572-8A26-1806417E87F0}" name="Item name "/>
@@ -471,8 +505,8 @@
     <tableColumn id="4" xr3:uid="{7D2095D8-7620-4899-8687-050E610BE7DF}" name="Description"/>
     <tableColumn id="5" xr3:uid="{F9570E16-0713-4961-B3C1-47CACC1A0467}" name="Supplier"/>
     <tableColumn id="6" xr3:uid="{0185D33D-A6C7-4940-A199-F8F5DC0199F8}" name="Quantity "/>
-    <tableColumn id="7" xr3:uid="{C21C8143-3C50-4801-A363-425817E6C503}" name="Unit price" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{F04832B8-365F-44B9-95D9-5C6F85186917}" name="Total price" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{C21C8143-3C50-4801-A363-425817E6C503}" name="Unit price" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{F04832B8-365F-44B9-95D9-5C6F85186917}" name="Total price" dataDxfId="15">
       <calculatedColumnFormula>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{A7DAB8C0-5901-40BC-909B-A19B354C0654}" name="Link"/>
@@ -778,11 +812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20442AE5-CF60-48D9-8E45-32FAF571F881}">
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20442AE5-CF60-48D9-8E45-32FAF571F881}">
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,27 +824,27 @@
     <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" customWidth="1"/>
+    <col min="10" max="10" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2">
         <f>SUM(H4:H43)</f>
-        <v>4096</v>
+        <v>415.40999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -850,26 +884,26 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>110.48</v>
+        <v>25.53</v>
       </c>
       <c r="H4" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>2762</v>
+        <v>25.53</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>12</v>
@@ -877,425 +911,464 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
       <c r="F5">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
-        <v>7.72</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="H5" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>1158</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="10">
         <v>30456389</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="H6" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>24.48</v>
+      </c>
       <c r="H7" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>24.48</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="7"/>
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>12.24</v>
+      </c>
       <c r="H8" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>12.24</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="12"/>
-      <c r="D9" s="7"/>
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>20</v>
+      </c>
       <c r="H9" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="8"/>
-      <c r="D10" s="7"/>
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>28.72</v>
+      </c>
       <c r="H10" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="7"/>
+        <v>28.72</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="11"/>
-      <c r="D11" s="7"/>
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>16.61</v>
+      </c>
       <c r="H11" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>16.61</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="12"/>
-      <c r="D12" s="7"/>
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>14.31</v>
+      </c>
       <c r="H12" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="7"/>
+        <v>14.31</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>43.46</v>
+      </c>
       <c r="H13" s="2">
         <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="14"/>
+        <v>43.46</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="16"/>
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="7"/>
-      <c r="H14" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="15"/>
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="12"/>
-      <c r="H15" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="12"/>
       <c r="D16" s="7"/>
-      <c r="H16" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C17" s="12"/>
       <c r="D17" s="7"/>
-      <c r="H17" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
       <c r="D18" s="7"/>
-      <c r="H18" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
-      <c r="H19" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="H20" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13"/>
+      <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C21" s="12"/>
       <c r="D21" s="7"/>
-      <c r="H21" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" s="7"/>
-      <c r="H22" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
       <c r="D23" s="7"/>
-      <c r="H23" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
-      <c r="H24" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="14"/>
-      <c r="H25" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D26" s="7"/>
-      <c r="H26" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C27" s="8"/>
       <c r="D27" s="7"/>
-      <c r="H27" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
       <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H28" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H29" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H30" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H31" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H32" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H36" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H37" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H38" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H39" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H40" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H41" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H42" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H43" s="2">
-        <f>Table2[[#This Row],[Quantity ]]*Table2[[#This Row],[Unit price]]</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="F4:I4 F5:H5 D6:H7 A8:H8 A9:B12 B13 D9:H12 F13:H13 D14:I14 D15 F15:I15 A14:B16 D16:I16 E17:E18 B17:B21 A4:B7 D4:D5">
-    <cfRule type="expression" dxfId="11" priority="16">
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="F4:I4 F5:H5 E17:E18 B17:B21 D4:D5 D6:H7 C10:D10 A16:B16 F10:I10 D8:D9 F8:H9 E8:E10 A4:B10 D11:H11 A11:A12 E12:H13 D12 A14:A15 D14:I16">
+    <cfRule type="expression" dxfId="14" priority="25">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="13" priority="23">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="12" priority="19">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:B27">
     <cfRule type="expression" dxfId="8" priority="10">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B15">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:B27">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{50BCA967-3FA4-4CD4-B5EC-DF97BB2BFB14}"/>
-    <hyperlink ref="D4" location="Sheet1!A1" tooltip="Silver Aluminium Profile Strut, 30 x 60 mm, 8mm Groove, 3000mm Length" display="Aluminum extrusion " xr:uid="{C32BCDAD-F70F-41D5-9EA1-A7102E366327}"/>
+    <hyperlink ref="D4" location="Arena!A1" tooltip="Silver Aluminium Profile Strut, 30 x 30 mm, 8mm Groove, 1000mm Length" display="Aluminum extrusion " xr:uid="{C32BCDAD-F70F-41D5-9EA1-A7102E366327}"/>
     <hyperlink ref="I5" r:id="rId2" xr:uid="{76164332-D8A5-41D5-BED0-4B81ADBA901F}"/>
     <hyperlink ref="D5" location="Sheet1!A1" tooltip="M6 Angle Bracket Connecting Component, Strut Profile 30 mm, Groove Size 8mm" display="Angle bracket" xr:uid="{8C1A59BD-26CB-4EB7-9A2D-1CF9AA0D6D27}"/>
     <hyperlink ref="D6" location="Sheet1!A1" tooltip="Ohaus Navigator Model NVT2201 2200g x 0.1g Portable Balance" display="Scale" xr:uid="{CBBC2BA5-1A31-458C-9170-1221D8008BCA}"/>
     <hyperlink ref="I6" r:id="rId3" xr:uid="{60AC8B77-9F34-40AE-AB3C-5172F259963D}"/>
+    <hyperlink ref="D11" location="Arena!A1" tooltip="RS PRO M6 x 25mm Hex Socket Cap Screw Plain Stainless Steel" display="Cap screw M6 25mm" xr:uid="{B84C6E22-0F03-4511-9A8B-E5517F2AB344}"/>
+    <hyperlink ref="D7" location="Arena!A1" tooltip="Acrylic Red tinted 5mm Sheet 730mm x 430mm " display="Acrylic red tinted 5mm" xr:uid="{B5BCEA37-CF87-4125-8A3E-56B9CFF89712}"/>
+    <hyperlink ref="D8" location="Arena!A1" tooltip="Acrylic Clear 2mm Sheet 730mm x 430mm" display="Acrylic clear 2mm" xr:uid="{21328F1A-507A-4639-BFEF-0A5F0AB99F62}"/>
+    <hyperlink ref="D10" location="Arena!A1" tooltip="Acrylic White Mat 5mm Sheet 730mm x 430mm" display="Acrylic white matt 5mm" xr:uid="{06B93EB5-C34F-4142-B607-C4FC60A082AF}"/>
+    <hyperlink ref="D9" location="Arena!A1" tooltip="Acrylic White MAtt 3mm Sheet 730mm x 430mm" display="Acrylic white matt 3mm" xr:uid="{5B060C5F-C154-40B5-871D-F94EA3B8A9A3}"/>
+    <hyperlink ref="I11" r:id="rId4" display="Cap screw M6 25mm" xr:uid="{4552FA82-D4A4-4353-8C8D-FF05E86FF820}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{A0AEAF26-9EA4-45AC-A2B8-0EAB8F17DD8F}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{2DD924A0-0F83-423C-A9EF-0B70AB865C42}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{69546910-D384-43E2-88A7-9813A0525B15}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{D335F4FC-0D2A-4FD4-BD1B-57BF88C15C64}"/>
+    <hyperlink ref="D12" location="Arena!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M6 x 12mm" display="Countersunk screw M6 12mm" xr:uid="{58FC70C6-5482-4A6D-9661-9CA52FE2082A}"/>
+    <hyperlink ref="D13" location="Arena!A1" tooltip="RS PRO M6 x 50mm Hex Socket Cap Screw Plain Stainless Steel" display="Cap screw M6 50mm" xr:uid="{525571B6-BEE7-4129-8DDB-064A3E7D7F54}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{64921401-0E84-48DE-9721-4BF7AE4624B3}"/>
+    <hyperlink ref="I13" r:id="rId10" xr:uid="{08181BAD-16D9-4E75-A722-D9EE9C5AF997}"/>
+    <hyperlink ref="I14" r:id="rId11" xr:uid="{79221C75-D184-4777-9A16-2DE25A946C78}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{FF46DEA7-5C88-47E1-8C9B-498229670596}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>